<commit_message>
added logs from 12.08
</commit_message>
<xml_diff>
--- a/data/daily_logs.xlsx
+++ b/data/daily_logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://komaralliance-my.sharepoint.com/personal/dshao_komar_com/Documents/Production Logs/September 2025/streamlit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="508" documentId="8_{EA7A99F6-1694-487A-9FFB-F46B9189E3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E50DF5FD-7162-416A-B069-2D22752B8086}"/>
+  <xr:revisionPtr revIDLastSave="578" documentId="8_{EA7A99F6-1694-487A-9FFB-F46B9189E3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7ACDF849-53A3-4761-BD4C-DA65D627C964}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-12660" windowWidth="16440" windowHeight="28320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4580" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4784" uniqueCount="77">
   <si>
     <t>Production Output</t>
   </si>
@@ -346,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -380,6 +380,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3284,7 +3285,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Shift/ Machine">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Shift/ Machine">
   <location ref="A21:E46" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" dataField="1" showAll="0" sortType="descending">
@@ -3470,7 +3471,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000001000000}" name="PivotTable5" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Machine">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000001000000}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Machine">
   <location ref="A5:E18" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" dataField="1" showAll="0" sortType="descending">
@@ -3984,12 +3985,12 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -4240,12 +4241,12 @@
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
     </row>
     <row r="21" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
@@ -7231,11 +7232,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G959"/>
+  <dimension ref="A1:G1010"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A920" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E958" sqref="E958"/>
+      <pane ySplit="1" topLeftCell="A969" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E977" sqref="E977"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29276,7 +29277,7 @@
         <v>24</v>
       </c>
       <c r="D943" s="21" t="str">
-        <f t="shared" ref="D943:D959" si="29">TEXT(B943, "dddd")</f>
+        <f t="shared" ref="D943:D993" si="29">TEXT(B943, "dddd")</f>
         <v>Friday</v>
       </c>
       <c r="E943" s="21">
@@ -29666,6 +29667,1210 @@
         <v>40</v>
       </c>
       <c r="G959" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="960" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A960" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B960" s="2">
+        <v>45985</v>
+      </c>
+      <c r="C960" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D960" s="22" t="str">
+        <f t="shared" ref="D960:D976" si="30">TEXT(B960, "dddd")</f>
+        <v>Monday</v>
+      </c>
+      <c r="E960" s="22">
+        <v>5220</v>
+      </c>
+      <c r="F960" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G960" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="961" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A961" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B961" s="2">
+        <v>45985</v>
+      </c>
+      <c r="C961" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D961" s="22" t="str">
+        <f t="shared" si="30"/>
+        <v>Monday</v>
+      </c>
+      <c r="E961" s="22">
+        <v>4307</v>
+      </c>
+      <c r="F961" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G961" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="962" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A962" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B962" s="2">
+        <v>45985</v>
+      </c>
+      <c r="C962" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D962" s="22" t="str">
+        <f t="shared" si="30"/>
+        <v>Monday</v>
+      </c>
+      <c r="E962" s="22">
+        <v>3652</v>
+      </c>
+      <c r="F962" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G962" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="963" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A963" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B963" s="2">
+        <v>45985</v>
+      </c>
+      <c r="C963" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D963" s="22" t="str">
+        <f t="shared" si="30"/>
+        <v>Monday</v>
+      </c>
+      <c r="E963" s="22">
+        <v>352</v>
+      </c>
+      <c r="F963" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G963" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="964" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A964" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B964" s="2">
+        <v>45985</v>
+      </c>
+      <c r="C964" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D964" s="22" t="str">
+        <f t="shared" si="30"/>
+        <v>Monday</v>
+      </c>
+      <c r="E964" s="22">
+        <v>1985</v>
+      </c>
+      <c r="F964" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G964" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="965" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A965" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B965" s="2">
+        <v>45985</v>
+      </c>
+      <c r="C965" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D965" s="22" t="str">
+        <f t="shared" si="30"/>
+        <v>Monday</v>
+      </c>
+      <c r="E965" s="22">
+        <v>1378</v>
+      </c>
+      <c r="F965" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G965" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="966" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A966" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B966" s="2">
+        <v>45985</v>
+      </c>
+      <c r="C966" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D966" s="22" t="str">
+        <f t="shared" si="30"/>
+        <v>Monday</v>
+      </c>
+      <c r="E966" s="22">
+        <v>4965</v>
+      </c>
+      <c r="F966" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G966" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="967" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A967" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B967" s="2">
+        <v>45985</v>
+      </c>
+      <c r="C967" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D967" s="22" t="str">
+        <f t="shared" si="30"/>
+        <v>Monday</v>
+      </c>
+      <c r="E967" s="22">
+        <v>6945</v>
+      </c>
+      <c r="F967" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G967" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="968" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A968" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B968" s="2">
+        <v>45985</v>
+      </c>
+      <c r="C968" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D968" s="22" t="str">
+        <f t="shared" si="30"/>
+        <v>Monday</v>
+      </c>
+      <c r="E968" s="22">
+        <v>4352</v>
+      </c>
+      <c r="F968" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G968" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="969" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A969" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B969" s="2">
+        <v>45985</v>
+      </c>
+      <c r="C969" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D969" s="22" t="str">
+        <f t="shared" si="30"/>
+        <v>Monday</v>
+      </c>
+      <c r="F969" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="G969" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="970" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A970" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B970" s="2">
+        <v>45985</v>
+      </c>
+      <c r="C970" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D970" s="22" t="str">
+        <f t="shared" si="30"/>
+        <v>Monday</v>
+      </c>
+      <c r="E970" s="22">
+        <v>11760</v>
+      </c>
+      <c r="F970" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G970" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="971" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A971" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B971" s="2">
+        <v>45985</v>
+      </c>
+      <c r="C971" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D971" s="22" t="str">
+        <f t="shared" si="30"/>
+        <v>Monday</v>
+      </c>
+      <c r="E971" s="22">
+        <v>7492</v>
+      </c>
+      <c r="F971" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G971" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="972" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A972" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B972" s="2">
+        <v>45985</v>
+      </c>
+      <c r="C972" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D972" s="22" t="str">
+        <f t="shared" si="30"/>
+        <v>Monday</v>
+      </c>
+      <c r="E972" s="22">
+        <v>17386</v>
+      </c>
+      <c r="F972" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G972" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="973" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A973" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B973" s="2">
+        <v>45985</v>
+      </c>
+      <c r="C973" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D973" s="22" t="str">
+        <f t="shared" si="30"/>
+        <v>Monday</v>
+      </c>
+      <c r="E973" s="22">
+        <v>17483</v>
+      </c>
+      <c r="F973" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G973" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="974" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A974" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B974" s="2">
+        <v>45985</v>
+      </c>
+      <c r="C974" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D974" s="22" t="str">
+        <f t="shared" si="30"/>
+        <v>Monday</v>
+      </c>
+      <c r="E974" s="22">
+        <v>2843</v>
+      </c>
+      <c r="F974" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G974" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="975" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A975" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B975" s="2">
+        <v>45985</v>
+      </c>
+      <c r="C975" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D975" s="22" t="str">
+        <f t="shared" si="30"/>
+        <v>Monday</v>
+      </c>
+      <c r="E975" s="22">
+        <v>7315</v>
+      </c>
+      <c r="F975" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G975" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="976" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A976" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B976" s="2">
+        <v>45985</v>
+      </c>
+      <c r="C976" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D976" s="22" t="str">
+        <f t="shared" si="30"/>
+        <v>Monday</v>
+      </c>
+      <c r="E976" s="22">
+        <v>4349</v>
+      </c>
+      <c r="F976" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G976" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="977" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A977" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B977" s="2">
+        <v>45986</v>
+      </c>
+      <c r="C977" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D977" s="22" t="str">
+        <f t="shared" si="29"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="E977" s="22">
+        <v>2376</v>
+      </c>
+      <c r="F977" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G977" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="978" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A978" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B978" s="2">
+        <v>45986</v>
+      </c>
+      <c r="C978" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D978" s="22" t="str">
+        <f t="shared" si="29"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="E978" s="22">
+        <v>7459</v>
+      </c>
+      <c r="F978" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G978" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="979" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A979" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B979" s="2">
+        <v>45986</v>
+      </c>
+      <c r="C979" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D979" s="22" t="str">
+        <f t="shared" si="29"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="E979" s="22">
+        <v>2527</v>
+      </c>
+      <c r="F979" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G979" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="980" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A980" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B980" s="2">
+        <v>45986</v>
+      </c>
+      <c r="C980" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D980" s="22" t="str">
+        <f t="shared" si="29"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="E980" s="22">
+        <v>279</v>
+      </c>
+      <c r="F980" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G980" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="981" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A981" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B981" s="2">
+        <v>45986</v>
+      </c>
+      <c r="C981" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D981" s="22" t="str">
+        <f t="shared" si="29"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="E981" s="22">
+        <v>447</v>
+      </c>
+      <c r="F981" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G981" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="982" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A982" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B982" s="2">
+        <v>45986</v>
+      </c>
+      <c r="C982" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D982" s="22" t="str">
+        <f t="shared" si="29"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="E982" s="22">
+        <v>2394</v>
+      </c>
+      <c r="F982" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G982" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="983" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A983" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B983" s="2">
+        <v>45986</v>
+      </c>
+      <c r="C983" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D983" s="22" t="str">
+        <f t="shared" si="29"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="E983" s="22">
+        <v>6120</v>
+      </c>
+      <c r="F983" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G983" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="984" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A984" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B984" s="2">
+        <v>45986</v>
+      </c>
+      <c r="C984" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D984" s="22" t="str">
+        <f t="shared" si="29"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="E984" s="22">
+        <v>8160</v>
+      </c>
+      <c r="F984" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G984" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="985" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A985" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B985" s="2">
+        <v>45986</v>
+      </c>
+      <c r="C985" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D985" s="22" t="str">
+        <f t="shared" si="29"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="F985" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="G985" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="986" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A986" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B986" s="2">
+        <v>45986</v>
+      </c>
+      <c r="C986" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D986" s="22" t="str">
+        <f t="shared" si="29"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="F986" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="G986" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="987" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A987" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B987" s="2">
+        <v>45986</v>
+      </c>
+      <c r="C987" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D987" s="22" t="str">
+        <f t="shared" si="29"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="F987" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="G987" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="988" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A988" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B988" s="2">
+        <v>45986</v>
+      </c>
+      <c r="C988" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D988" s="22" t="str">
+        <f t="shared" si="29"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="E988" s="22">
+        <v>6682</v>
+      </c>
+      <c r="F988" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G988" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="989" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A989" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B989" s="2">
+        <v>45986</v>
+      </c>
+      <c r="C989" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D989" s="22" t="str">
+        <f t="shared" si="29"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="E989" s="22">
+        <v>20578</v>
+      </c>
+      <c r="F989" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G989" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="990" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A990" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B990" s="2">
+        <v>45986</v>
+      </c>
+      <c r="C990" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D990" s="22" t="str">
+        <f t="shared" si="29"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="E990" s="22">
+        <v>17054</v>
+      </c>
+      <c r="F990" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G990" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="991" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A991" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B991" s="2">
+        <v>45986</v>
+      </c>
+      <c r="C991" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D991" s="22" t="str">
+        <f t="shared" si="29"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="E991" s="22">
+        <v>1270</v>
+      </c>
+      <c r="F991" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G991" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="992" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A992" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B992" s="2">
+        <v>45986</v>
+      </c>
+      <c r="C992" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D992" s="22" t="str">
+        <f t="shared" si="29"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="E992" s="22">
+        <v>6603</v>
+      </c>
+      <c r="F992" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G992" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="993" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A993" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B993" s="2">
+        <v>45986</v>
+      </c>
+      <c r="C993" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D993" s="22" t="str">
+        <f t="shared" si="29"/>
+        <v>Tuesday</v>
+      </c>
+      <c r="E993" s="22">
+        <v>2470</v>
+      </c>
+      <c r="F993" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G993" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="994" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A994" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B994" s="2">
+        <v>45987</v>
+      </c>
+      <c r="C994" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D994" s="22" t="str">
+        <f t="shared" ref="D994:D1010" si="31">TEXT(B994, "dddd")</f>
+        <v>Wednesday</v>
+      </c>
+      <c r="E994" s="22">
+        <v>2637</v>
+      </c>
+      <c r="F994" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G994" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="995" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A995" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B995" s="2">
+        <v>45987</v>
+      </c>
+      <c r="C995" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D995" s="22" t="str">
+        <f t="shared" si="31"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E995" s="22">
+        <v>6712</v>
+      </c>
+      <c r="F995" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G995" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="996" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A996" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B996" s="2">
+        <v>45987</v>
+      </c>
+      <c r="C996" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D996" s="22" t="str">
+        <f t="shared" si="31"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E996" s="22">
+        <v>2860</v>
+      </c>
+      <c r="F996" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G996" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="997" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A997" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B997" s="2">
+        <v>45987</v>
+      </c>
+      <c r="C997" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D997" s="22" t="str">
+        <f t="shared" si="31"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E997" s="22">
+        <v>2434</v>
+      </c>
+      <c r="F997" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="G997" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="998" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A998" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B998" s="2">
+        <v>45987</v>
+      </c>
+      <c r="C998" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D998" s="22" t="str">
+        <f t="shared" si="31"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E998" s="22">
+        <v>2639</v>
+      </c>
+      <c r="F998" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G998" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="999" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A999" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B999" s="2">
+        <v>45987</v>
+      </c>
+      <c r="C999" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D999" s="22" t="str">
+        <f t="shared" si="31"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E999" s="22"/>
+      <c r="F999" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="G999" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1000" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1000" s="2">
+        <v>45987</v>
+      </c>
+      <c r="C1000" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1000" s="22" t="str">
+        <f t="shared" si="31"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E1000" s="22">
+        <v>6161</v>
+      </c>
+      <c r="F1000" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1000" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1001" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1001" s="2">
+        <v>45987</v>
+      </c>
+      <c r="C1001" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1001" s="22" t="str">
+        <f t="shared" si="31"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E1001" s="22">
+        <v>6320</v>
+      </c>
+      <c r="F1001" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1001" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1002" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1002" s="2">
+        <v>45987</v>
+      </c>
+      <c r="C1002" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1002" s="22" t="str">
+        <f t="shared" si="31"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E1002" s="22">
+        <v>6928</v>
+      </c>
+      <c r="F1002" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1002" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1003" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1003" s="2">
+        <v>45987</v>
+      </c>
+      <c r="C1003" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1003" s="22" t="str">
+        <f t="shared" si="31"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E1003" s="22"/>
+      <c r="F1003" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1003" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1004" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1004" s="2">
+        <v>45987</v>
+      </c>
+      <c r="C1004" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1004" s="22" t="str">
+        <f t="shared" si="31"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E1004" s="22"/>
+      <c r="F1004" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1004" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1005" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1005" s="2">
+        <v>45987</v>
+      </c>
+      <c r="C1005" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1005" s="22" t="str">
+        <f t="shared" si="31"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E1005" s="22">
+        <v>5093</v>
+      </c>
+      <c r="F1005" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1005" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1006" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1006" s="2">
+        <v>45987</v>
+      </c>
+      <c r="C1006" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1006" s="22" t="str">
+        <f t="shared" si="31"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E1006" s="22">
+        <v>8381</v>
+      </c>
+      <c r="F1006" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1006" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1007" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1007" s="2">
+        <v>45987</v>
+      </c>
+      <c r="C1007" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1007" s="22" t="str">
+        <f t="shared" si="31"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E1007" s="22">
+        <v>19444</v>
+      </c>
+      <c r="F1007" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1007" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1008" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1008" s="2">
+        <v>45987</v>
+      </c>
+      <c r="C1008" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1008" s="22" t="str">
+        <f t="shared" si="31"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E1008" s="22"/>
+      <c r="F1008" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1008" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1009" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1009" s="2">
+        <v>45987</v>
+      </c>
+      <c r="C1009" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1009" s="22" t="str">
+        <f t="shared" si="31"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E1009" s="22">
+        <v>2418</v>
+      </c>
+      <c r="F1009" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1009" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1010" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1010" s="2">
+        <v>45987</v>
+      </c>
+      <c r="C1010" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1010" s="22" t="str">
+        <f t="shared" si="31"/>
+        <v>Wednesday</v>
+      </c>
+      <c r="E1010" s="22">
+        <v>3800</v>
+      </c>
+      <c r="F1010" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1010" s="22" t="s">
         <v>40</v>
       </c>
     </row>
@@ -29905,7 +31110,7 @@
         <v>70.5</v>
       </c>
       <c r="C25" s="21">
-        <f t="shared" ref="C25:C31" si="1">A25*B25</f>
+        <f t="shared" ref="C25:C28" si="1">A25*B25</f>
         <v>2256</v>
       </c>
     </row>

</xml_diff>